<commit_message>
updated Scrum file for info regarding User stories 1,10 for sprint 1
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anerishah/Desktop/SSW555/PROJECTS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikdeo/Desktop/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E0473A-2B6F-BC4B-9AF2-8290D7BF6579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ACD96B-307F-114A-A1CE-CF9A5550477B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="21000" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27220" windowHeight="17540" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,18 +23,10 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -44,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="220">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -731,6 +723,9 @@
   </si>
   <si>
     <t>Project03_CS555.py</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -2197,7 +2192,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
+  <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3104,8 +3099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3186,13 +3181,13 @@
         <v>201</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>218</v>
@@ -3354,6 +3349,12 @@
       </c>
       <c r="C11" t="s">
         <v>201</v>
+      </c>
+      <c r="D11" t="s">
+        <v>219</v>
+      </c>
+      <c r="F11">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.15">
@@ -3387,13 +3388,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -3422,6 +3426,34 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3481,7 +3513,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3525,8 +3557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B41"/>
+    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
updated information for sprint 1
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikdeo/Desktop/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ACD96B-307F-114A-A1CE-CF9A5550477B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914AC2F0-B7A7-844A-8EC9-E4DBBC522718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27220" windowHeight="17540" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27220" windowHeight="17540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="220">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2214,7 +2214,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2257,7 +2257,7 @@
         <v>201</v>
       </c>
       <c r="E2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -2397,6 +2397,9 @@
       <c r="D11" t="s">
         <v>201</v>
       </c>
+      <c r="E11" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
@@ -2465,10 +2468,13 @@
         <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+        <v>201</v>
+      </c>
+      <c r="E16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2479,10 +2485,13 @@
         <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+        <v>201</v>
+      </c>
+      <c r="E17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2496,7 +2505,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2510,7 +2519,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2524,7 +2533,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2538,7 +2547,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2566,7 +2575,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2580,7 +2589,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2594,7 +2603,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2608,7 +2617,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2636,7 +2645,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2650,7 +2659,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2678,7 +2687,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3021,7 +3030,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3099,7 +3108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -3390,7 +3399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3399,7 +3408,7 @@
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
updated PD user stories with helper functions
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikdeo/Desktop/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914AC2F0-B7A7-844A-8EC9-E4DBBC522718}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC99EDD-2D24-7E40-81DC-E3A46D5533E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27220" windowHeight="17540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="220">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3108,7 +3108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -3474,10 +3474,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3509,6 +3509,22 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3519,10 +3535,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3554,6 +3570,22 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated sprint 2 status
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS 555\abc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meetk\Documents\Python Scripts\ssw555tmDammp2020spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACB07AB-3915-4D7D-946A-8E7A7CCAA73B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CE4E68-934D-42C6-B620-8E816B661EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="1044" windowWidth="19452" windowHeight="10536" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2173,7 +2173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -3952,8 +3952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4041,7 +4041,7 @@
         <v>204</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -4121,7 +4121,7 @@
         <v>187</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E8">
         <v>35</v>
@@ -4141,7 +4141,7 @@
         <v>204</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E9">
         <v>25</v>
@@ -4627,7 +4627,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
updated PD user story 15, 16 for sprint 2
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahirdhall/Desktop/CS 555/ssw555tmDammp2020spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikdeo/Desktop/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB82FEF-53C6-A045-A13F-8F485105F7DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49F3A25-766D-0C4C-A4F0-6E53A78D551E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16400" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$A$1:$E$41</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2299,7 +2293,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
+  <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3959,7 +3953,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4104,6 +4098,15 @@
       <c r="F6">
         <v>45</v>
       </c>
+      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6" s="24">
+        <v>42430</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -4123,6 +4126,15 @@
       </c>
       <c r="F7">
         <v>40</v>
+      </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+      <c r="I7" s="24">
+        <v>42430</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -4684,7 +4696,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
updated errors and gedcom
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepkakadia/ssw555tmDammp2020spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anerishah/Desktop/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4A74CE-40AB-FE42-8269-A980B443758C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17B91CF-7F53-F54F-BB1B-AD618BCC7465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="257">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2360,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2574,7 +2574,7 @@
         <v>202</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -2727,7 +2727,7 @@
         <v>202</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -2744,7 +2744,7 @@
         <v>200</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -2761,7 +2761,7 @@
         <v>200</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -2778,7 +2778,7 @@
         <v>203</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -2795,7 +2795,7 @@
         <v>186</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -2846,7 +2846,7 @@
         <v>186</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -2863,7 +2863,7 @@
         <v>203</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -2880,7 +2880,7 @@
         <v>200</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -2896,8 +2896,8 @@
       <c r="D31" t="s">
         <v>201</v>
       </c>
-      <c r="E31" t="s">
-        <v>218</v>
+      <c r="E31" s="20" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -2914,7 +2914,7 @@
         <v>200</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -2931,7 +2931,7 @@
         <v>201</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -2948,7 +2948,7 @@
         <v>203</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -2965,7 +2965,7 @@
         <v>186</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -2982,7 +2982,7 @@
         <v>201</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -2999,7 +2999,7 @@
         <v>202</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -3016,7 +3016,7 @@
         <v>186</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -3033,7 +3033,7 @@
         <v>203</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -3049,8 +3049,8 @@
       <c r="D40" t="s">
         <v>201</v>
       </c>
-      <c r="E40" t="s">
-        <v>218</v>
+      <c r="E40" s="20" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -3065,6 +3065,9 @@
       </c>
       <c r="D41" t="s">
         <v>202</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -4040,7 +4043,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4112,13 +4115,19 @@
         <v>202</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E2">
         <v>25</v>
       </c>
       <c r="F2">
         <v>30</v>
+      </c>
+      <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
       </c>
       <c r="I2" s="24">
         <v>42445</v>
@@ -4154,7 +4163,7 @@
         <v>201</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -4202,7 +4211,7 @@
         <v>203</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -4442,7 +4451,7 @@
         <v>203</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E9">
         <v>25</v>
@@ -4490,7 +4499,7 @@
         <v>201</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E10">
         <v>30</v>
@@ -4538,7 +4547,7 @@
         <v>202</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E11">
         <v>35</v>

</xml_diff>

<commit_message>
updated sprint 3 for PD in spreadsheet
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahirdhall/Desktop/CS 555/ssw555tmDammp2020spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikdeo/Desktop/project/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF4961D-35A6-0B43-A2EA-FD76232030ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6E4337-4FD5-9342-ADAF-F437D2BA9A58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16340" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$D$1:$D$41</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2343,7 +2337,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
+  <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4635,8 +4629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4692,6 +4686,15 @@
       <c r="F2">
         <v>40</v>
       </c>
+      <c r="G2">
+        <v>24</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" s="24">
+        <v>42456</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3">
@@ -4711,6 +4714,15 @@
       </c>
       <c r="F3">
         <v>40</v>
+      </c>
+      <c r="G3">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>35</v>
+      </c>
+      <c r="I3" s="24">
+        <v>42456</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -5075,7 +5087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="101" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="101" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated for sprint 4
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anerishah/Desktop/ssw555tmDammp2020spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meetk\Documents\Python Scripts\ssw555tmDammp2020spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A12DC37-348E-9F43-856C-C412831401FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EC6E03-49E4-4CD0-829B-64CE886F4C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16340" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="1044" windowWidth="19452" windowHeight="10536" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="271">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -883,6 +883,12 @@
   </si>
   <si>
     <t>Merging of code should be done early to detect errors</t>
+  </si>
+  <si>
+    <t>test_us38</t>
+  </si>
+  <si>
+    <t>test_us33</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1038,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1076,6 +1082,7 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1185,7 +1192,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42416</c:v>
@@ -1256,7 +1263,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1345,7 +1352,7 @@
             <c:numRef>
               <c:f>Burndown!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42416</c:v>
@@ -1411,7 +1418,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2255,16 +2262,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2281,7 +2288,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -2298,7 +2305,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -2315,7 +2322,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2332,7 +2339,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -2349,7 +2356,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -2366,7 +2373,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
@@ -2400,16 +2407,16 @@
       <selection activeCell="B41" sqref="B41:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="30.5" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -2426,7 +2433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2443,7 +2450,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2460,7 +2467,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2477,7 +2484,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2494,7 +2501,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2511,7 +2518,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2528,7 +2535,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2545,7 +2552,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2562,7 +2569,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2579,7 +2586,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2596,7 +2603,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2613,7 +2620,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2630,7 +2637,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2647,7 +2654,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2664,7 +2671,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2681,7 +2688,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2698,7 +2705,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2715,7 +2722,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2732,7 +2739,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2749,7 +2756,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2766,7 +2773,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2783,7 +2790,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2800,7 +2807,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2817,7 +2824,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2834,7 +2841,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2851,7 +2858,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2868,7 +2875,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2885,7 +2892,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2902,7 +2909,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2919,7 +2926,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2936,7 +2943,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2953,7 +2960,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2970,7 +2977,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2987,7 +2994,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3004,7 +3011,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3021,7 +3028,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3038,7 +3045,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3055,7 +3062,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3072,7 +3079,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3089,7 +3096,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3121,47 +3128,47 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>155</v>
       </c>
@@ -3184,7 +3191,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>156</v>
       </c>
@@ -3200,7 +3207,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>157</v>
       </c>
@@ -3225,7 +3232,7 @@
         <v>42.105263157894733</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>158</v>
       </c>
@@ -3250,7 +3257,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>159</v>
       </c>
@@ -3275,7 +3282,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>160</v>
       </c>
@@ -3315,17 +3322,17 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>155</v>
       </c>
@@ -3348,7 +3355,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>156</v>
       </c>
@@ -3364,7 +3371,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -3389,7 +3396,7 @@
         <v>42.105263157894733</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>158</v>
       </c>
@@ -3413,7 +3420,7 @@
         <v>62.500000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>159</v>
       </c>
@@ -3437,7 +3444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>160</v>
       </c>
@@ -3478,27 +3485,27 @@
       <selection activeCell="B15" sqref="B15:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" style="17" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" style="17" customWidth="1"/>
+    <col min="12" max="12" width="19.1796875" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" style="17" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.6328125" style="17" customWidth="1"/>
+    <col min="16" max="16" width="16.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3545,7 +3552,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -3592,7 +3599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -3639,7 +3646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -3686,7 +3693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -3733,7 +3740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>208</v>
       </c>
@@ -3780,7 +3787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -3827,7 +3834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -3874,7 +3881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>211</v>
       </c>
@@ -3921,7 +3928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>212</v>
       </c>
@@ -3968,7 +3975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -4015,53 +4022,53 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="M12" s="18"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>214</v>
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="22" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="22" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B20" s="22" t="s">
         <v>229</v>
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="22" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="22" t="s">
         <v>228</v>
       </c>
@@ -4077,21 +4084,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.83203125" customWidth="1"/>
-    <col min="11" max="11" width="19.5" customWidth="1"/>
-    <col min="12" max="12" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" customWidth="1"/>
+    <col min="12" max="12" width="21.453125" customWidth="1"/>
+    <col min="13" max="13" width="14.6328125" customWidth="1"/>
+    <col min="15" max="15" width="17.36328125" customWidth="1"/>
+    <col min="16" max="16" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4139,7 +4146,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -4187,7 +4194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -4235,7 +4242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -4283,7 +4290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -4331,7 +4338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -4379,7 +4386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -4427,7 +4434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -4475,7 +4482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -4523,7 +4530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>126</v>
       </c>
@@ -4571,7 +4578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>127</v>
       </c>
@@ -4619,39 +4626,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="22"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="22"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="22"/>
     </row>
-    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="22" t="s">
         <v>254</v>
       </c>
@@ -4667,19 +4674,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView topLeftCell="H1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.36328125" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="32.33203125" customWidth="1"/>
-    <col min="15" max="15" width="23.83203125" customWidth="1"/>
+    <col min="12" max="12" width="32.36328125" customWidth="1"/>
+    <col min="15" max="15" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4727,7 +4734,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>21</v>
       </c>
@@ -4775,7 +4782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>22</v>
       </c>
@@ -4823,7 +4830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>23</v>
       </c>
@@ -4871,7 +4878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
@@ -4919,7 +4926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>25</v>
       </c>
@@ -4967,7 +4974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>26</v>
       </c>
@@ -5015,7 +5022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>27</v>
       </c>
@@ -5063,7 +5070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>28</v>
       </c>
@@ -5111,7 +5118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>32</v>
       </c>
@@ -5159,7 +5166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>30</v>
       </c>
@@ -5207,39 +5214,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="22"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="22"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="22"/>
     </row>
-    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B24" s="22" t="s">
         <v>268</v>
       </c>
@@ -5252,18 +5259,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.36328125" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -5291,8 +5299,27 @@
       <c r="I1" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K1" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -5311,8 +5338,21 @@
       <c r="F2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K2" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -5331,8 +5371,21 @@
       <c r="F3">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K3" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -5343,7 +5396,7 @@
         <v>203</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -5351,8 +5404,36 @@
       <c r="F4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4" s="25">
+        <v>42434</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="M4" s="18">
+        <v>25</v>
+      </c>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -5371,8 +5452,21 @@
       <c r="F5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K5" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -5391,8 +5485,21 @@
       <c r="F6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K6" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -5411,8 +5518,21 @@
       <c r="F7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K7" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -5431,8 +5551,21 @@
       <c r="F8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K8" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -5443,7 +5576,7 @@
         <v>203</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E9">
         <v>25</v>
@@ -5451,8 +5584,36 @@
       <c r="F9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G9">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>25</v>
+      </c>
+      <c r="I9" s="25">
+        <v>42434</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="M9" s="18">
+        <v>25</v>
+      </c>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -5471,8 +5632,21 @@
       <c r="F10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K10" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -5490,6 +5664,19 @@
       </c>
       <c r="F11">
         <v>25</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5502,17 +5689,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="139" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B43" sqref="A43:B43"/>
+    <sheetView topLeftCell="A33" zoomScale="139" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>107</v>
       </c>
@@ -5523,7 +5710,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -5534,7 +5721,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -5545,7 +5732,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -5556,7 +5743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -5567,7 +5754,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -5578,7 +5765,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -5589,7 +5776,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -5600,7 +5787,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -5611,7 +5798,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -5622,7 +5809,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -5633,7 +5820,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -5644,7 +5831,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -5655,7 +5842,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -5666,7 +5853,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -5677,7 +5864,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -5688,7 +5875,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -5699,7 +5886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -5710,7 +5897,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -5721,7 +5908,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -5732,7 +5919,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -5743,7 +5930,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -5754,7 +5941,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -5765,7 +5952,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -5776,7 +5963,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -5787,7 +5974,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -5798,7 +5985,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>133</v>
       </c>
@@ -5809,7 +5996,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -5820,7 +6007,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -5831,7 +6018,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -5842,7 +6029,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -5853,7 +6040,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>138</v>
       </c>
@@ -5864,7 +6051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>139</v>
       </c>
@@ -5875,7 +6062,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>140</v>
       </c>
@@ -5886,7 +6073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>141</v>
       </c>
@@ -5897,7 +6084,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>142</v>
       </c>
@@ -5908,7 +6095,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>143</v>
       </c>
@@ -5919,7 +6106,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -5930,7 +6117,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>145</v>
       </c>
@@ -5941,7 +6128,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -5952,7 +6139,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -5963,7 +6150,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>148</v>
       </c>
@@ -5974,7 +6161,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
Completed Sprint 4 Mahir
us34 and us37 updated excel sprint info
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meetk\Documents\Python Scripts\ssw555tmDammp2020spring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahirdhall/Desktop/CS 555/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EC6E03-49E4-4CD0-829B-64CE886F4C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4D260D-B7CB-CA43-9A17-C65EFE083C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="1044" windowWidth="19452" windowHeight="10536" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="1040" windowWidth="25940" windowHeight="14440" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$D$1:$D$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Sprint4!$C$1:$C$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,9 +35,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="275">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -889,6 +888,18 @@
   </si>
   <si>
     <t>test_us33</t>
+  </si>
+  <si>
+    <t>test_us37</t>
+  </si>
+  <si>
+    <t>test_us34</t>
+  </si>
+  <si>
+    <t>us34</t>
+  </si>
+  <si>
+    <t>us37</t>
   </si>
 </sst>
 </file>
@@ -899,7 +910,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -944,6 +955,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1038,7 +1055,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1083,6 +1100,7 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1192,7 +1210,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42416</c:v>
@@ -1263,7 +1281,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1352,7 +1370,7 @@
             <c:numRef>
               <c:f>Burndown!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42416</c:v>
@@ -1418,7 +1436,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2262,16 +2280,16 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2288,7 +2306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -2305,7 +2323,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>201</v>
       </c>
@@ -2322,7 +2340,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2339,7 +2357,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>202</v>
       </c>
@@ -2356,7 +2374,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>203</v>
       </c>
@@ -2373,7 +2391,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>30</v>
       </c>
@@ -2403,20 +2421,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:C41"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="30.453125" customWidth="1"/>
-    <col min="4" max="4" width="8.81640625" customWidth="1"/>
+    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -2433,7 +2451,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2450,7 +2468,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2467,7 +2485,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2484,7 +2502,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2501,7 +2519,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2518,7 +2536,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2535,7 +2553,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2552,7 +2570,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2569,7 +2587,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2586,7 +2604,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2603,7 +2621,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2620,7 +2638,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2637,7 +2655,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2654,7 +2672,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2671,7 +2689,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2688,7 +2706,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2705,7 +2723,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2722,7 +2740,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2739,7 +2757,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2756,7 +2774,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2773,7 +2791,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2790,7 +2808,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2807,7 +2825,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2824,7 +2842,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2841,7 +2859,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2858,7 +2876,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2875,7 +2893,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2892,7 +2910,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2909,7 +2927,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2926,7 +2944,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2943,7 +2961,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2960,7 +2978,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2977,7 +2995,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2994,7 +3012,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3008,10 +3026,10 @@
         <v>186</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3028,7 +3046,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>4</v>
       </c>
@@ -3045,7 +3063,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3059,10 +3077,10 @@
         <v>186</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3079,7 +3097,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3096,7 +3114,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3128,47 +3146,47 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="16.36328125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>155</v>
       </c>
@@ -3191,7 +3209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>156</v>
       </c>
@@ -3207,7 +3225,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>157</v>
       </c>
@@ -3232,7 +3250,7 @@
         <v>42.105263157894733</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>158</v>
       </c>
@@ -3257,7 +3275,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>159</v>
       </c>
@@ -3282,7 +3300,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>160</v>
       </c>
@@ -3322,17 +3340,17 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>155</v>
       </c>
@@ -3355,7 +3373,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>156</v>
       </c>
@@ -3371,7 +3389,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -3396,7 +3414,7 @@
         <v>42.105263157894733</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>158</v>
       </c>
@@ -3420,7 +3438,7 @@
         <v>62.500000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>159</v>
       </c>
@@ -3444,7 +3462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>160</v>
       </c>
@@ -3485,27 +3503,27 @@
       <selection activeCell="B15" sqref="B15:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.453125" style="17" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="17" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="19.6328125" style="17" customWidth="1"/>
-    <col min="16" max="16" width="16.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" style="17" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3552,7 +3570,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -3599,7 +3617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -3646,7 +3664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -3693,7 +3711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -3740,7 +3758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>208</v>
       </c>
@@ -3787,7 +3805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -3834,7 +3852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -3881,7 +3899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>211</v>
       </c>
@@ -3928,7 +3946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>212</v>
       </c>
@@ -3975,7 +3993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -4022,53 +4040,53 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="M12" s="18"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>214</v>
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B17" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="22" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="22" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B20" s="22" t="s">
         <v>229</v>
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B21" s="22" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="22" t="s">
         <v>228</v>
       </c>
@@ -4088,17 +4106,17 @@
       <selection activeCell="B15" sqref="B15:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="29.81640625" customWidth="1"/>
-    <col min="11" max="11" width="19.453125" customWidth="1"/>
-    <col min="12" max="12" width="21.453125" customWidth="1"/>
-    <col min="13" max="13" width="14.6328125" customWidth="1"/>
-    <col min="15" max="15" width="17.36328125" customWidth="1"/>
-    <col min="16" max="16" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="11" max="11" width="19.5" customWidth="1"/>
+    <col min="12" max="12" width="21.5" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4146,7 +4164,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -4194,7 +4212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -4242,7 +4260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -4290,7 +4308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -4338,7 +4356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -4386,7 +4404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -4434,7 +4452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -4482,7 +4500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -4530,7 +4548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>126</v>
       </c>
@@ -4578,7 +4596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>127</v>
       </c>
@@ -4626,39 +4644,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B17" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B19" s="22"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="22"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" s="22"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B22" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="22" t="s">
         <v>254</v>
       </c>
@@ -4674,19 +4692,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:Q11"/>
+    <sheetView topLeftCell="M1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="24.36328125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="32.36328125" customWidth="1"/>
-    <col min="15" max="15" width="23.81640625" customWidth="1"/>
+    <col min="12" max="12" width="32.33203125" customWidth="1"/>
+    <col min="15" max="15" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4734,7 +4752,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>21</v>
       </c>
@@ -4782,7 +4800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>22</v>
       </c>
@@ -4830,7 +4848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>23</v>
       </c>
@@ -4878,7 +4896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>24</v>
       </c>
@@ -4926,7 +4944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>25</v>
       </c>
@@ -4974,7 +4992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>26</v>
       </c>
@@ -5022,7 +5040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>27</v>
       </c>
@@ -5070,7 +5088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>28</v>
       </c>
@@ -5118,7 +5136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>32</v>
       </c>
@@ -5166,7 +5184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>30</v>
       </c>
@@ -5214,39 +5232,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B20" s="22"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B21" s="22"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" s="22"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B24" s="22" t="s">
         <v>268</v>
       </c>
@@ -5261,17 +5279,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.36328125" customWidth="1"/>
-    <col min="12" max="12" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -5319,7 +5340,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -5352,7 +5373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -5385,7 +5406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -5433,7 +5454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -5452,21 +5473,36 @@
       <c r="F5">
         <v>30</v>
       </c>
+      <c r="G5">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+      <c r="I5" s="24">
+        <v>42475</v>
+      </c>
       <c r="K5" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="L5" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="M5">
+        <v>40</v>
+      </c>
       <c r="N5" s="18"/>
       <c r="O5" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="P5" s="18"/>
+      <c r="P5" s="26" t="s">
+        <v>272</v>
+      </c>
       <c r="Q5" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -5499,7 +5535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -5532,7 +5568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>144</v>
       </c>
@@ -5551,21 +5587,36 @@
       <c r="F8">
         <v>30</v>
       </c>
+      <c r="G8">
+        <v>44</v>
+      </c>
+      <c r="H8">
+        <v>50</v>
+      </c>
+      <c r="I8" s="24">
+        <v>42475</v>
+      </c>
       <c r="K8" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
+      <c r="L8" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="M8">
+        <v>40</v>
+      </c>
       <c r="N8" s="18"/>
       <c r="O8" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="P8" s="18"/>
+      <c r="P8" s="26" t="s">
+        <v>271</v>
+      </c>
       <c r="Q8" s="18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -5613,7 +5664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>146</v>
       </c>
@@ -5646,7 +5697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -5689,17 +5740,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="139" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A34" zoomScale="139" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>107</v>
       </c>
@@ -5710,7 +5761,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -5721,7 +5772,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -5732,7 +5783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -5743,7 +5794,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -5754,7 +5805,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -5765,7 +5816,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -5776,7 +5827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -5787,7 +5838,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>115</v>
       </c>
@@ -5798,7 +5849,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -5809,7 +5860,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>117</v>
       </c>
@@ -5820,7 +5871,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>118</v>
       </c>
@@ -5831,7 +5882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -5842,7 +5893,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -5853,7 +5904,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -5864,7 +5915,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -5875,7 +5926,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>123</v>
       </c>
@@ -5886,7 +5937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>124</v>
       </c>
@@ -5897,7 +5948,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -5908,7 +5959,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -5919,7 +5970,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -5930,7 +5981,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -5941,7 +5992,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -5952,7 +6003,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -5963,7 +6014,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -5974,7 +6025,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>132</v>
       </c>
@@ -5985,7 +6036,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>133</v>
       </c>
@@ -5996,7 +6047,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -6007,7 +6058,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -6018,7 +6069,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>136</v>
       </c>
@@ -6029,7 +6080,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>137</v>
       </c>
@@ -6040,7 +6091,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>138</v>
       </c>
@@ -6051,7 +6102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>139</v>
       </c>
@@ -6062,7 +6113,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>140</v>
       </c>
@@ -6073,7 +6124,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>141</v>
       </c>
@@ -6084,7 +6135,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>142</v>
       </c>
@@ -6095,7 +6146,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>143</v>
       </c>
@@ -6106,7 +6157,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -6117,7 +6168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>145</v>
       </c>
@@ -6128,7 +6179,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>146</v>
       </c>
@@ -6139,7 +6190,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -6150,7 +6201,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>148</v>
       </c>
@@ -6161,7 +6212,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
updated user stories and test cases for PD for sprint 4
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahirdhall/Desktop/CS 555/ssw555tmDammp2020spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikdeo/Desktop/project/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4D260D-B7CB-CA43-9A17-C65EFE083C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDF383-01E3-D944-9689-91540F22926E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="1040" windowWidth="25940" windowHeight="14440" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,16 +27,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$D$1:$D$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Sprint4!$C$1:$C$11</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -46,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="279">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -900,6 +894,18 @@
   </si>
   <si>
     <t>us37</t>
+  </si>
+  <si>
+    <t>us29</t>
+  </si>
+  <si>
+    <t>us31</t>
+  </si>
+  <si>
+    <t>test_us29</t>
+  </si>
+  <si>
+    <t>test_us31</t>
   </si>
 </sst>
 </file>
@@ -2400,7 +2406,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
+  <sortState ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4692,7 +4698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -5279,8 +5285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5359,18 +5365,33 @@
       <c r="F2">
         <v>20</v>
       </c>
+      <c r="G2">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>45</v>
+      </c>
+      <c r="I2" s="24">
+        <v>42476</v>
+      </c>
       <c r="K2" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="L2" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="M2" s="18">
+        <v>17</v>
+      </c>
       <c r="N2" s="18"/>
       <c r="O2" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="P2" s="18"/>
+      <c r="P2" s="18" t="s">
+        <v>277</v>
+      </c>
       <c r="Q2" s="18">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
@@ -5392,18 +5413,33 @@
       <c r="F3">
         <v>25</v>
       </c>
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>45</v>
+      </c>
+      <c r="I3" s="24">
+        <v>42476</v>
+      </c>
       <c r="K3" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="L3" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="M3" s="18">
+        <v>18</v>
+      </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="P3" s="18"/>
+      <c r="P3" s="18" t="s">
+        <v>278</v>
+      </c>
       <c r="Q3" s="18">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Sprint-4 updated burndown and sprint 4
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pratikdeo/Desktop/project/ssw555tmDammp2020spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepkakadia/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDF383-01E3-D944-9689-91540F22926E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBAD004-F741-E346-9600-E99D0605A9A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1040" windowWidth="25940" windowHeight="14440" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6380" yWindow="2600" windowWidth="25940" windowHeight="14440" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backlog!$D$1:$D$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Sprint4!$C$1:$C$11</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="284">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -761,9 +769,6 @@
     <t>Adding files in gitignore to avoid any clashes</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
     <t>test_cases/test.py</t>
   </si>
   <si>
@@ -906,6 +911,24 @@
   </si>
   <si>
     <t>test_us31</t>
+  </si>
+  <si>
+    <t>us39</t>
+  </si>
+  <si>
+    <t>us38</t>
+  </si>
+  <si>
+    <t>us33</t>
+  </si>
+  <si>
+    <t>40-45</t>
+  </si>
+  <si>
+    <t>test_us39</t>
+  </si>
+  <si>
+    <t>test_us35</t>
   </si>
 </sst>
 </file>
@@ -1391,7 +1414,7 @@
                   <c:v>42493</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>42507</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2406,7 +2429,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:D5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D5">
     <sortCondition ref="C3:C5"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2427,8 +2450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A25" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2451,7 +2474,7 @@
         <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>27</v>
@@ -2947,7 +2970,7 @@
         <v>200</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -2981,7 +3004,7 @@
         <v>200</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -3015,7 +3038,7 @@
         <v>203</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -3049,7 +3072,7 @@
         <v>201</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -3066,7 +3089,7 @@
         <v>202</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -3100,7 +3123,7 @@
         <v>203</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -3117,7 +3140,7 @@
         <v>201</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -3134,7 +3157,7 @@
         <v>202</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -3342,8 +3365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3472,8 +3495,8 @@
       <c r="A6" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>230</v>
+      <c r="B6" s="23">
+        <v>42507</v>
       </c>
       <c r="C6" s="14">
         <v>0</v>
@@ -3483,14 +3506,14 @@
         <v>10</v>
       </c>
       <c r="E6" s="14">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="F6" s="15">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="G6" s="9">
         <f>(E6-E5)/F6*60</f>
-        <v>-30000</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3614,10 +3637,10 @@
         <v>219</v>
       </c>
       <c r="O2" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="P2" s="18" t="s">
         <v>231</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>232</v>
       </c>
       <c r="Q2" s="18">
         <v>4</v>
@@ -3661,10 +3684,10 @@
         <v>219</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q3" s="18">
         <v>4</v>
@@ -3708,10 +3731,10 @@
         <v>219</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P4" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q4" s="18">
         <v>4</v>
@@ -3755,10 +3778,10 @@
         <v>219</v>
       </c>
       <c r="O5" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q5" s="18">
         <v>4</v>
@@ -3802,10 +3825,10 @@
         <v>219</v>
       </c>
       <c r="O6" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q6" s="18">
         <v>4</v>
@@ -3849,10 +3872,10 @@
         <v>219</v>
       </c>
       <c r="O7" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q7" s="18">
         <v>4</v>
@@ -3896,10 +3919,10 @@
         <v>219</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q8" s="18">
         <v>4</v>
@@ -3943,10 +3966,10 @@
         <v>219</v>
       </c>
       <c r="O9" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q9" s="18">
         <v>4</v>
@@ -3990,10 +4013,10 @@
         <v>219</v>
       </c>
       <c r="O10" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q10" s="18">
         <v>4</v>
@@ -4037,10 +4060,10 @@
         <v>219</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q11" s="18">
         <v>4</v>
@@ -4161,7 +4184,7 @@
       </c>
       <c r="N1" s="17"/>
       <c r="O1" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>176</v>
@@ -4209,10 +4232,10 @@
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q2" s="18">
         <v>4</v>
@@ -4257,10 +4280,10 @@
       </c>
       <c r="N3" s="17"/>
       <c r="O3" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q3" s="18">
         <v>4</v>
@@ -4305,10 +4328,10 @@
       </c>
       <c r="N4" s="17"/>
       <c r="O4" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P4" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q4" s="18">
         <v>4</v>
@@ -4353,10 +4376,10 @@
       </c>
       <c r="N5" s="17"/>
       <c r="O5" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q5" s="18">
         <v>4</v>
@@ -4401,10 +4424,10 @@
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q6" s="18">
         <v>4</v>
@@ -4449,10 +4472,10 @@
       </c>
       <c r="N7" s="17"/>
       <c r="O7" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q7" s="18">
         <v>4</v>
@@ -4497,10 +4520,10 @@
       </c>
       <c r="N8" s="17"/>
       <c r="O8" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q8" s="18">
         <v>4</v>
@@ -4545,10 +4568,10 @@
       </c>
       <c r="N9" s="17"/>
       <c r="O9" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q9" s="18">
         <v>4</v>
@@ -4593,10 +4616,10 @@
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q10" s="18">
         <v>4</v>
@@ -4641,10 +4664,10 @@
       </c>
       <c r="N11" s="17"/>
       <c r="O11" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q11" s="18">
         <v>4</v>
@@ -4665,7 +4688,7 @@
     </row>
     <row r="18" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.15">
@@ -4684,7 +4707,7 @@
     </row>
     <row r="23" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -4698,8 +4721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="H1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="M11" sqref="M2:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4749,7 +4772,7 @@
       </c>
       <c r="N1" s="18"/>
       <c r="O1" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P1" s="18" t="s">
         <v>176</v>
@@ -4769,7 +4792,7 @@
         <v>200</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -4797,10 +4820,10 @@
       </c>
       <c r="N2" s="18"/>
       <c r="O2" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q2" s="18">
         <v>4</v>
@@ -4817,7 +4840,7 @@
         <v>200</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3">
         <v>15</v>
@@ -4845,10 +4868,10 @@
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q3" s="18">
         <v>4</v>
@@ -4865,7 +4888,7 @@
         <v>203</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -4893,10 +4916,10 @@
       </c>
       <c r="N4" s="18"/>
       <c r="O4" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P4" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q4" s="18">
         <v>4</v>
@@ -4913,7 +4936,7 @@
         <v>186</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -4941,10 +4964,10 @@
       </c>
       <c r="N5" s="18"/>
       <c r="O5" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q5" s="18">
         <v>4</v>
@@ -4961,7 +4984,7 @@
         <v>202</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -4989,10 +5012,10 @@
       </c>
       <c r="N6" s="18"/>
       <c r="O6" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q6" s="18">
         <v>4</v>
@@ -5009,7 +5032,7 @@
         <v>202</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -5037,10 +5060,10 @@
       </c>
       <c r="N7" s="18"/>
       <c r="O7" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q7" s="18">
         <v>4</v>
@@ -5057,7 +5080,7 @@
         <v>186</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -5085,10 +5108,10 @@
       </c>
       <c r="N8" s="18"/>
       <c r="O8" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q8" s="18">
         <v>4</v>
@@ -5105,7 +5128,7 @@
         <v>203</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E9">
         <v>20</v>
@@ -5133,10 +5156,10 @@
       </c>
       <c r="N9" s="18"/>
       <c r="O9" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Q9" s="18">
         <v>4</v>
@@ -5153,7 +5176,7 @@
         <v>201</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E10">
         <v>20</v>
@@ -5181,10 +5204,10 @@
       </c>
       <c r="N10" s="18"/>
       <c r="O10" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Q10" s="18">
         <v>4</v>
@@ -5201,7 +5224,7 @@
         <v>201</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E11">
         <v>20</v>
@@ -5229,10 +5252,10 @@
       </c>
       <c r="N11" s="18"/>
       <c r="O11" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Q11" s="18">
         <v>4</v>
@@ -5253,7 +5276,7 @@
     </row>
     <row r="19" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
@@ -5272,7 +5295,7 @@
     </row>
     <row r="24" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B24" s="22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -5285,8 +5308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5337,7 +5360,7 @@
       </c>
       <c r="N1" s="18"/>
       <c r="O1" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P1" s="18" t="s">
         <v>176</v>
@@ -5378,17 +5401,17 @@
         <v>217</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="M2" s="18">
-        <v>17</v>
+        <v>274</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>281</v>
       </c>
       <c r="N2" s="18"/>
       <c r="O2" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q2" s="18">
         <v>10</v>
@@ -5426,17 +5449,17 @@
         <v>217</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="M3" s="18">
-        <v>18</v>
+        <v>275</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>281</v>
       </c>
       <c r="N3" s="18"/>
       <c r="O3" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Q3" s="18">
         <v>12</v>
@@ -5474,17 +5497,17 @@
         <v>217</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="M4" s="18">
-        <v>25</v>
+        <v>280</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>281</v>
       </c>
       <c r="N4" s="18"/>
       <c r="O4" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P4" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q4" s="18">
         <v>18</v>
@@ -5522,17 +5545,17 @@
         <v>217</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="M5">
-        <v>40</v>
+        <v>272</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>281</v>
       </c>
       <c r="N5" s="18"/>
       <c r="O5" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q5" s="18">
         <v>4</v>
@@ -5561,12 +5584,16 @@
         <v>217</v>
       </c>
       <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="M6" s="18" t="s">
+        <v>281</v>
+      </c>
       <c r="N6" s="18"/>
       <c r="O6" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="P6" s="18"/>
+        <v>230</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>283</v>
+      </c>
       <c r="Q6" s="18">
         <v>4</v>
       </c>
@@ -5594,10 +5621,12 @@
         <v>217</v>
       </c>
       <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="M7" s="18" t="s">
+        <v>281</v>
+      </c>
       <c r="N7" s="18"/>
       <c r="O7" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P7" s="18"/>
       <c r="Q7" s="18">
@@ -5636,17 +5665,17 @@
         <v>217</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="M8">
-        <v>40</v>
+        <v>273</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>281</v>
       </c>
       <c r="N8" s="18"/>
       <c r="O8" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P8" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="Q8" s="18">
         <v>14</v>
@@ -5684,17 +5713,17 @@
         <v>217</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="M9" s="18">
-        <v>25</v>
+        <v>279</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>281</v>
       </c>
       <c r="N9" s="18"/>
       <c r="O9" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Q9" s="18">
         <v>15</v>
@@ -5719,16 +5748,31 @@
       <c r="F10">
         <v>20</v>
       </c>
+      <c r="G10">
+        <v>35</v>
+      </c>
+      <c r="H10">
+        <v>25</v>
+      </c>
+      <c r="I10" s="25">
+        <v>42431</v>
+      </c>
       <c r="K10" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
+      <c r="L10" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>281</v>
+      </c>
       <c r="N10" s="18"/>
       <c r="O10" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="P10" s="18"/>
+        <v>230</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>282</v>
+      </c>
       <c r="Q10" s="18">
         <v>4</v>
       </c>
@@ -5759,7 +5803,7 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="P11" s="18"/>
       <c r="Q11" s="18">
@@ -6198,7 +6242,7 @@
         <v>144</v>
       </c>
       <c r="B38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
updated US 42 and team report
</commit_message>
<xml_diff>
--- a/ASDKMDMPPD.xlsx
+++ b/ASDKMDMPPD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anerishah/Desktop/ssw555tmDammp2020spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DB19FD-E248-324D-9FCE-75A1FB856338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD17A43F-687D-D540-9864-BFD708B91503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="2600" windowWidth="25940" windowHeight="14440" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6380" yWindow="2600" windowWidth="25940" windowHeight="14440" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2462,7 +2462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="150" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -3540,7 +3540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:B23"/>
     </sheetView>
   </sheetViews>
@@ -4733,8 +4733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="M11" sqref="M2:M11"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5320,7 +5320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -5871,7 +5871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="139" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A38" zoomScale="139" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>

</xml_diff>